<commit_message>
Adding new sex variable
</commit_message>
<xml_diff>
--- a/data/final_data/manually_cleaned_data.xlsx
+++ b/data/final_data/manually_cleaned_data.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahgross/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahgross/Desktop/W241/Final Project/Olive_Oil_Taste_Test/data/final_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D2D91E-01BA-294C-B19C-5502E2EC02FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CD54E9-3CA0-EF47-81FE-8BD6E1BDCCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="500" windowWidth="18940" windowHeight="14900" xr2:uid="{49F459C7-6492-B94F-B44D-4BE8CD6D4D26}"/>
+    <workbookView xWindow="10180" yWindow="600" windowWidth="18940" windowHeight="14900" xr2:uid="{49F459C7-6492-B94F-B44D-4BE8CD6D4D26}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="Only Tested" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All!$A$1:$T$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All!$A$1:$U$97</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="235">
   <si>
     <t>admin</t>
   </si>
@@ -741,6 +741,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>sex</t>
   </si>
 </sst>
 </file>
@@ -771,18 +774,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -800,9 +797,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1118,11 +1115,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADBB74E-D12A-8C49-88BF-474E0A7757AC}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:T97"/>
+  <dimension ref="A1:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1132,19 +1131,19 @@
     <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" customWidth="1"/>
-    <col min="22" max="22" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -1182,32 +1181,35 @@
         <v>1</v>
       </c>
       <c r="M1" t="s">
-        <v>2</v>
+        <v>234</v>
       </c>
       <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>114</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>113</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -1234,20 +1236,20 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
         <v>156</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>157</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>110</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -1255,9 +1257,12 @@
       <c r="T2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="U2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
@@ -1282,32 +1287,35 @@
         <v>172</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>156</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>157</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>111</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
       <c r="R3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
@@ -1340,30 +1348,33 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>156</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>157</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>111</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
@@ -1388,32 +1399,35 @@
         <v>159</v>
       </c>
       <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
         <v>156</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>157</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>110</v>
       </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
       <c r="R5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
@@ -1438,22 +1452,22 @@
         <v>155</v>
       </c>
       <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
         <v>156</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>157</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>111</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
       <c r="R6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <v>2</v>
@@ -1461,9 +1475,12 @@
       <c r="T6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="U6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
@@ -1488,32 +1505,35 @@
         <v>163</v>
       </c>
       <c r="M7">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
         <v>156</v>
       </c>
-      <c r="O7" t="s">
-        <v>154</v>
-      </c>
       <c r="P7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q7" t="s">
         <v>111</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="s">
         <v>112</v>
       </c>
-      <c r="S7">
-        <v>2</v>
-      </c>
       <c r="T7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
@@ -1540,30 +1560,33 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
         <v>156</v>
       </c>
-      <c r="O8" t="s">
-        <v>154</v>
-      </c>
       <c r="P8" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q8" t="s">
         <v>111</v>
       </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
       <c r="R8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
@@ -1588,31 +1611,34 @@
         <v>159</v>
       </c>
       <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
         <v>156</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>157</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>111</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
       <c r="R9">
         <v>1</v>
       </c>
       <c r="S9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1631,29 +1657,29 @@
       <c r="H10" t="s">
         <v>154</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>158</v>
       </c>
       <c r="L10" t="s">
         <v>159</v>
       </c>
       <c r="M10">
-        <v>2</v>
-      </c>
-      <c r="N10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
         <v>160</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>157</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>110</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
       <c r="R10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <v>2</v>
@@ -1661,8 +1687,11 @@
       <c r="T10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1690,20 +1719,20 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>157</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>110</v>
       </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
       <c r="R11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S11">
         <v>2</v>
@@ -1711,8 +1740,11 @@
       <c r="T11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1737,8 +1769,8 @@
       <c r="H12" t="s">
         <v>154</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
         <v>221</v>
       </c>
       <c r="K12">
@@ -1748,31 +1780,34 @@
         <v>159</v>
       </c>
       <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
         <v>156</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>157</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>110</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
       <c r="R12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1797,8 +1832,8 @@
       <c r="H13" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
         <v>222</v>
       </c>
       <c r="K13">
@@ -1810,29 +1845,32 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
         <v>156</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>157</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>110</v>
       </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
       <c r="R13">
         <v>1</v>
       </c>
       <c r="S13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1852,38 +1890,41 @@
         <v>159</v>
       </c>
       <c r="M14">
-        <v>2</v>
-      </c>
-      <c r="N14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="O14" t="s">
-        <v>154</v>
-      </c>
       <c r="P14" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q14" t="s">
         <v>111</v>
       </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
       <c r="R14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E15">
@@ -1904,29 +1945,32 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="O15" t="s">
-        <v>154</v>
-      </c>
       <c r="P15" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q15" t="s">
         <v>110</v>
       </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
       <c r="R15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1954,29 +1998,32 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>157</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>110</v>
       </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
       <c r="R16">
-        <v>2</v>
-      </c>
-      <c r="S16" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="T16" t="s">
         <v>112</v>
       </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1998,29 +2045,32 @@
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>157</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>111</v>
       </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
       <c r="R17">
         <v>1</v>
       </c>
       <c r="S17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2039,29 +2089,29 @@
       <c r="H18" t="s">
         <v>154</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="1" t="s">
         <v>161</v>
       </c>
       <c r="L18" t="s">
         <v>159</v>
       </c>
       <c r="M18">
-        <v>2</v>
-      </c>
-      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18" t="s">
         <v>156</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>157</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>111</v>
       </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
       <c r="R18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -2069,8 +2119,11 @@
       <c r="T18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2089,29 +2142,29 @@
       <c r="H19" t="s">
         <v>154</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="1" t="s">
         <v>162</v>
       </c>
       <c r="L19" t="s">
         <v>163</v>
       </c>
       <c r="M19">
-        <v>2</v>
-      </c>
-      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19" t="s">
         <v>164</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>157</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>111</v>
       </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
       <c r="R19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S19">
         <v>2</v>
@@ -2119,8 +2172,11 @@
       <c r="T19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="U19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2133,14 +2189,14 @@
       <c r="F20" t="s">
         <v>106</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>110</v>
       </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2153,14 +2209,14 @@
       <c r="F21" t="s">
         <v>106</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>110</v>
       </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2173,14 +2229,14 @@
       <c r="F22" t="s">
         <v>106</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>110</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2193,14 +2249,14 @@
       <c r="F23" t="s">
         <v>106</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>111</v>
       </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2213,14 +2269,14 @@
       <c r="F24" t="s">
         <v>106</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>111</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2233,14 +2289,14 @@
       <c r="F25" t="s">
         <v>106</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>111</v>
       </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2253,14 +2309,14 @@
       <c r="F26" t="s">
         <v>106</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>110</v>
       </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2273,14 +2329,14 @@
       <c r="F27" t="s">
         <v>106</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>110</v>
       </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2312,22 +2368,22 @@
         <v>155</v>
       </c>
       <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
         <v>165</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>157</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>110</v>
       </c>
-      <c r="Q28">
-        <v>1</v>
-      </c>
       <c r="R28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S28">
         <v>2</v>
@@ -2335,8 +2391,11 @@
       <c r="T28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2370,29 +2429,32 @@
       <c r="M29">
         <v>1</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
         <v>173</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>157</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>110</v>
       </c>
-      <c r="Q29">
-        <v>1</v>
-      </c>
       <c r="R29">
         <v>1</v>
       </c>
       <c r="S29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -2417,8 +2479,8 @@
       <c r="H30" t="s">
         <v>154</v>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2" t="s">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1" t="s">
         <v>223</v>
       </c>
       <c r="K30">
@@ -2428,31 +2490,34 @@
         <v>166</v>
       </c>
       <c r="M30">
-        <v>1</v>
-      </c>
-      <c r="N30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
         <v>160</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>157</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>111</v>
       </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
       <c r="R30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2477,38 +2542,41 @@
       <c r="H31" t="s">
         <v>154</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="1" t="s">
         <v>167</v>
       </c>
       <c r="L31" t="s">
         <v>159</v>
       </c>
       <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
         <v>3</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>160</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>157</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>111</v>
       </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
       <c r="R31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S31">
         <v>2</v>
       </c>
       <c r="T31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2533,27 +2601,27 @@
       <c r="H32" t="s">
         <v>154</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="1" t="s">
         <v>168</v>
       </c>
       <c r="L32" t="s">
         <v>159</v>
       </c>
       <c r="M32">
-        <v>0</v>
-      </c>
-      <c r="N32" t="s">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32" t="s">
         <v>160</v>
       </c>
-      <c r="O32" t="s">
-        <v>154</v>
-      </c>
       <c r="P32" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q32" t="s">
         <v>110</v>
       </c>
-      <c r="Q32">
-        <v>1</v>
-      </c>
       <c r="R32">
         <v>1</v>
       </c>
@@ -2561,10 +2629,13 @@
         <v>1</v>
       </c>
       <c r="T32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2589,7 +2660,7 @@
       <c r="H33" t="s">
         <v>154</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="1" t="s">
         <v>169</v>
       </c>
       <c r="L33" t="s">
@@ -2598,29 +2669,32 @@
       <c r="M33">
         <v>0</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
         <v>170</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>157</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>110</v>
       </c>
-      <c r="Q33">
-        <v>1</v>
-      </c>
       <c r="R33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2654,18 +2728,18 @@
       <c r="M34">
         <v>0</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
         <v>160</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>157</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>111</v>
       </c>
-      <c r="Q34">
-        <v>1</v>
-      </c>
       <c r="R34">
         <v>1</v>
       </c>
@@ -2673,10 +2747,13 @@
         <v>1</v>
       </c>
       <c r="T34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2701,38 +2778,41 @@
       <c r="H35" t="s">
         <v>154</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="1" t="s">
         <v>171</v>
       </c>
       <c r="L35" t="s">
         <v>172</v>
       </c>
       <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35" t="s">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35" t="s">
         <v>173</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>157</v>
       </c>
-      <c r="P35" t="s">
+      <c r="Q35" t="s">
         <v>110</v>
       </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
       <c r="R35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2757,7 +2837,7 @@
       <c r="H36" t="s">
         <v>154</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="1" t="s">
         <v>174</v>
       </c>
       <c r="L36" t="s">
@@ -2766,29 +2846,32 @@
       <c r="M36">
         <v>0</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
         <v>175</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>157</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>110</v>
       </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
       <c r="R36">
         <v>1</v>
       </c>
       <c r="S36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2813,38 +2896,41 @@
       <c r="H37" t="s">
         <v>154</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="1" t="s">
         <v>176</v>
       </c>
       <c r="L37" t="s">
         <v>163</v>
       </c>
       <c r="M37">
-        <v>1</v>
-      </c>
-      <c r="N37" t="s">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37" t="s">
         <v>160</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>157</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>111</v>
       </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
       <c r="R37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -2869,38 +2955,41 @@
       <c r="H38" t="s">
         <v>154</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="1" t="s">
         <v>177</v>
       </c>
       <c r="L38" t="s">
         <v>155</v>
       </c>
       <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38" t="s">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
         <v>160</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>157</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>110</v>
       </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="R38" t="s">
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38" t="s">
         <v>112</v>
       </c>
-      <c r="S38">
-        <v>2</v>
-      </c>
       <c r="T38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -2928,23 +3017,20 @@
       <c r="L39" t="s">
         <v>166</v>
       </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39" t="s">
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39" t="s">
         <v>178</v>
       </c>
-      <c r="O39" t="s">
-        <v>154</v>
-      </c>
       <c r="P39" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q39" t="s">
         <v>111</v>
       </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
       <c r="R39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S39">
         <v>2</v>
@@ -2952,8 +3038,11 @@
       <c r="T39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2982,31 +3071,34 @@
         <v>159</v>
       </c>
       <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40" t="s">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40" t="s">
         <v>160</v>
       </c>
-      <c r="O40" t="s">
-        <v>154</v>
-      </c>
       <c r="P40" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q40" t="s">
         <v>110</v>
       </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
       <c r="R40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -3031,27 +3123,27 @@
       <c r="H41" t="s">
         <v>154</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="1" t="s">
         <v>179</v>
       </c>
       <c r="L41" t="s">
         <v>159</v>
       </c>
       <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41" t="s">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41" t="s">
         <v>160</v>
       </c>
-      <c r="O41" t="s">
+      <c r="P41" t="s">
         <v>157</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>111</v>
       </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
       <c r="R41">
         <v>1</v>
       </c>
@@ -3059,10 +3151,13 @@
         <v>1</v>
       </c>
       <c r="T41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -3087,8 +3182,8 @@
       <c r="H42" t="s">
         <v>154</v>
       </c>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2" t="s">
+      <c r="I42" s="1"/>
+      <c r="J42" s="1" t="s">
         <v>224</v>
       </c>
       <c r="K42">
@@ -3098,31 +3193,34 @@
         <v>155</v>
       </c>
       <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42" t="s">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42" t="s">
         <v>160</v>
       </c>
-      <c r="O42" t="s">
+      <c r="P42" t="s">
         <v>157</v>
       </c>
-      <c r="P42" t="s">
+      <c r="Q42" t="s">
         <v>111</v>
       </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42" t="s">
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42" t="s">
         <v>112</v>
       </c>
-      <c r="S42">
-        <v>2</v>
-      </c>
       <c r="T42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -3147,7 +3245,7 @@
       <c r="H43" t="s">
         <v>154</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" s="1" t="s">
         <v>180</v>
       </c>
       <c r="L43" t="s">
@@ -3156,29 +3254,32 @@
       <c r="M43">
         <v>0</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43" t="s">
         <v>181</v>
       </c>
-      <c r="O43" t="s">
-        <v>154</v>
-      </c>
       <c r="P43" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q43" t="s">
         <v>110</v>
       </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
       <c r="R43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -3188,7 +3289,7 @@
       <c r="C44" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E44">
@@ -3203,7 +3304,7 @@
       <c r="H44" t="s">
         <v>154</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="J44" s="1" t="s">
         <v>150</v>
       </c>
       <c r="K44">
@@ -3215,29 +3316,32 @@
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="N44" t="s">
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" t="s">
         <v>160</v>
       </c>
-      <c r="O44" t="s">
-        <v>154</v>
-      </c>
       <c r="P44" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q44" t="s">
         <v>110</v>
       </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
       <c r="R44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -3262,7 +3366,7 @@
       <c r="H45" t="s">
         <v>154</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="J45" s="1" t="s">
         <v>182</v>
       </c>
       <c r="L45" t="s">
@@ -3271,29 +3375,32 @@
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45" t="s">
         <v>184</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>157</v>
       </c>
-      <c r="P45" t="s">
+      <c r="Q45" t="s">
         <v>110</v>
       </c>
-      <c r="Q45">
-        <v>1</v>
-      </c>
       <c r="R45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -3325,31 +3432,34 @@
         <v>159</v>
       </c>
       <c r="M46">
-        <v>0</v>
-      </c>
-      <c r="N46" t="s">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" t="s">
         <v>160</v>
       </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>157</v>
       </c>
-      <c r="P46" t="s">
+      <c r="Q46" t="s">
         <v>111</v>
       </c>
-      <c r="Q46">
-        <v>0</v>
-      </c>
       <c r="R46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -3374,27 +3484,27 @@
       <c r="H47" t="s">
         <v>154</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J47" s="1" t="s">
         <v>185</v>
       </c>
       <c r="L47" t="s">
         <v>186</v>
       </c>
       <c r="M47">
-        <v>0</v>
-      </c>
-      <c r="N47" t="s">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47" t="s">
         <v>160</v>
       </c>
-      <c r="O47" t="s">
+      <c r="P47" t="s">
         <v>157</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>111</v>
       </c>
-      <c r="Q47">
-        <v>1</v>
-      </c>
       <c r="R47">
         <v>1</v>
       </c>
@@ -3402,10 +3512,13 @@
         <v>1</v>
       </c>
       <c r="T47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -3430,29 +3543,29 @@
       <c r="H48" t="s">
         <v>154</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="1" t="s">
         <v>187</v>
       </c>
       <c r="L48" t="s">
         <v>155</v>
       </c>
       <c r="M48">
-        <v>0</v>
-      </c>
-      <c r="N48" t="s">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" t="s">
         <v>217</v>
       </c>
-      <c r="O48" t="s">
+      <c r="P48" t="s">
         <v>157</v>
       </c>
-      <c r="P48" t="s">
+      <c r="Q48" t="s">
         <v>111</v>
       </c>
-      <c r="Q48">
-        <v>0</v>
-      </c>
       <c r="R48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S48">
         <v>1</v>
@@ -3460,8 +3573,11 @@
       <c r="T48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -3486,38 +3602,41 @@
       <c r="H49" t="s">
         <v>154</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="J49" s="1" t="s">
         <v>188</v>
       </c>
       <c r="L49" t="s">
         <v>163</v>
       </c>
       <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49" t="s">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49" t="s">
         <v>160</v>
       </c>
-      <c r="O49" t="s">
+      <c r="P49" t="s">
         <v>157</v>
       </c>
-      <c r="P49" t="s">
+      <c r="Q49" t="s">
         <v>111</v>
       </c>
-      <c r="Q49">
-        <v>0</v>
-      </c>
       <c r="R49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -3542,7 +3661,7 @@
       <c r="H50" t="s">
         <v>154</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="J50" s="1" t="s">
         <v>189</v>
       </c>
       <c r="L50" t="s">
@@ -3551,18 +3670,18 @@
       <c r="M50">
         <v>0</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50" t="s">
         <v>218</v>
       </c>
-      <c r="O50" t="s">
-        <v>154</v>
-      </c>
       <c r="P50" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q50" t="s">
         <v>111</v>
       </c>
-      <c r="Q50">
-        <v>1</v>
-      </c>
       <c r="R50">
         <v>1</v>
       </c>
@@ -3570,10 +3689,13 @@
         <v>1</v>
       </c>
       <c r="T50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -3598,7 +3720,7 @@
       <c r="H51" t="s">
         <v>154</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="J51" s="1" t="s">
         <v>225</v>
       </c>
       <c r="K51">
@@ -3610,29 +3732,32 @@
       <c r="M51">
         <v>0</v>
       </c>
-      <c r="N51" t="s">
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51" t="s">
         <v>160</v>
       </c>
-      <c r="O51" t="s">
+      <c r="P51" t="s">
         <v>157</v>
       </c>
-      <c r="P51" t="s">
+      <c r="Q51" t="s">
         <v>111</v>
       </c>
-      <c r="Q51">
-        <v>1</v>
-      </c>
       <c r="R51">
         <v>1</v>
       </c>
       <c r="S51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -3657,27 +3782,27 @@
       <c r="H52" t="s">
         <v>154</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="J52" s="1" t="s">
         <v>190</v>
       </c>
       <c r="L52" t="s">
         <v>163</v>
       </c>
       <c r="M52">
-        <v>0</v>
-      </c>
-      <c r="N52" t="s">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52" t="s">
         <v>160</v>
       </c>
-      <c r="O52" t="s">
-        <v>154</v>
-      </c>
       <c r="P52" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q52" t="s">
         <v>110</v>
       </c>
-      <c r="Q52">
-        <v>1</v>
-      </c>
       <c r="R52">
         <v>1</v>
       </c>
@@ -3685,10 +3810,13 @@
         <v>1</v>
       </c>
       <c r="T52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -3713,7 +3841,7 @@
       <c r="H53" t="s">
         <v>154</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="J53" s="1" t="s">
         <v>191</v>
       </c>
       <c r="L53" t="s">
@@ -3722,29 +3850,32 @@
       <c r="M53">
         <v>0</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53" t="s">
         <v>160</v>
       </c>
-      <c r="O53" t="s">
+      <c r="P53" t="s">
         <v>157</v>
       </c>
-      <c r="P53" t="s">
+      <c r="Q53" t="s">
         <v>111</v>
       </c>
-      <c r="Q53">
-        <v>1</v>
-      </c>
       <c r="R53">
         <v>1</v>
       </c>
       <c r="S53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -3757,14 +3888,14 @@
       <c r="F54" t="s">
         <v>109</v>
       </c>
-      <c r="P54" t="s">
+      <c r="Q54" t="s">
         <v>111</v>
       </c>
-      <c r="Q54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -3777,14 +3908,14 @@
       <c r="F55" t="s">
         <v>109</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>111</v>
       </c>
-      <c r="Q55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -3809,38 +3940,41 @@
       <c r="H56" t="s">
         <v>154</v>
       </c>
-      <c r="J56" s="2" t="s">
+      <c r="J56" s="1" t="s">
         <v>192</v>
       </c>
       <c r="L56" t="s">
         <v>163</v>
       </c>
       <c r="M56">
-        <v>0</v>
-      </c>
-      <c r="N56" t="s">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56" t="s">
         <v>160</v>
       </c>
-      <c r="O56" t="s">
+      <c r="P56" t="s">
         <v>157</v>
       </c>
-      <c r="P56" t="s">
+      <c r="Q56" t="s">
         <v>110</v>
       </c>
-      <c r="Q56">
-        <v>1</v>
-      </c>
       <c r="R56">
         <v>1</v>
       </c>
       <c r="S56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -3865,7 +3999,7 @@
       <c r="H57" t="s">
         <v>154</v>
       </c>
-      <c r="J57" s="2" t="s">
+      <c r="J57" s="1" t="s">
         <v>193</v>
       </c>
       <c r="L57" t="s">
@@ -3874,29 +4008,32 @@
       <c r="M57">
         <v>0</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57" t="s">
         <v>160</v>
       </c>
-      <c r="O57" t="s">
+      <c r="P57" t="s">
         <v>157</v>
       </c>
-      <c r="P57" t="s">
+      <c r="Q57" t="s">
         <v>111</v>
       </c>
-      <c r="Q57">
-        <v>0</v>
-      </c>
       <c r="R57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -3921,8 +4058,8 @@
       <c r="H58" t="s">
         <v>154</v>
       </c>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2" t="s">
+      <c r="I58" s="1"/>
+      <c r="J58" s="1" t="s">
         <v>226</v>
       </c>
       <c r="K58">
@@ -3932,31 +4069,34 @@
         <v>159</v>
       </c>
       <c r="M58">
-        <v>0</v>
-      </c>
-      <c r="N58" t="s">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58" t="s">
         <v>160</v>
       </c>
-      <c r="O58" t="s">
-        <v>154</v>
-      </c>
       <c r="P58" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q58" t="s">
         <v>110</v>
       </c>
-      <c r="Q58">
-        <v>1</v>
-      </c>
       <c r="R58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -3990,29 +4130,32 @@
       <c r="M59">
         <v>0</v>
       </c>
-      <c r="N59" t="s">
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59" t="s">
         <v>160</v>
       </c>
-      <c r="O59" t="s">
+      <c r="P59" t="s">
         <v>157</v>
       </c>
-      <c r="P59" t="s">
+      <c r="Q59" t="s">
         <v>111</v>
       </c>
-      <c r="Q59">
-        <v>0</v>
-      </c>
       <c r="R59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -4037,7 +4180,7 @@
       <c r="H60" t="s">
         <v>154</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="J60" s="1" t="s">
         <v>194</v>
       </c>
       <c r="L60" t="s">
@@ -4046,29 +4189,32 @@
       <c r="M60">
         <v>0</v>
       </c>
-      <c r="N60" t="s">
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60" t="s">
         <v>160</v>
       </c>
-      <c r="O60" t="s">
+      <c r="P60" t="s">
         <v>157</v>
       </c>
-      <c r="P60" t="s">
+      <c r="Q60" t="s">
         <v>110</v>
       </c>
-      <c r="Q60">
-        <v>1</v>
-      </c>
       <c r="R60">
         <v>1</v>
       </c>
       <c r="S60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -4093,7 +4239,7 @@
       <c r="H61" t="s">
         <v>154</v>
       </c>
-      <c r="J61" s="2" t="s">
+      <c r="J61" s="1" t="s">
         <v>227</v>
       </c>
       <c r="K61">
@@ -4105,18 +4251,18 @@
       <c r="M61">
         <v>0</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61" t="s">
         <v>160</v>
       </c>
-      <c r="O61" t="s">
+      <c r="P61" t="s">
         <v>157</v>
       </c>
-      <c r="P61" t="s">
+      <c r="Q61" t="s">
         <v>110</v>
       </c>
-      <c r="Q61">
-        <v>1</v>
-      </c>
       <c r="R61">
         <v>1</v>
       </c>
@@ -4126,8 +4272,11 @@
       <c r="T61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -4152,7 +4301,7 @@
       <c r="H62" t="s">
         <v>157</v>
       </c>
-      <c r="J62" s="2" t="s">
+      <c r="J62" s="1" t="s">
         <v>195</v>
       </c>
       <c r="L62" t="s">
@@ -4161,29 +4310,32 @@
       <c r="M62">
         <v>0</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62" t="s">
         <v>165</v>
       </c>
-      <c r="O62" t="s">
-        <v>154</v>
-      </c>
       <c r="P62" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q62" t="s">
         <v>110</v>
       </c>
-      <c r="Q62">
-        <v>1</v>
-      </c>
       <c r="R62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -4215,31 +4367,34 @@
         <v>172</v>
       </c>
       <c r="M63">
-        <v>0</v>
-      </c>
-      <c r="N63" t="s">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63" t="s">
         <v>160</v>
       </c>
-      <c r="O63" t="s">
+      <c r="P63" t="s">
         <v>157</v>
       </c>
-      <c r="P63" t="s">
+      <c r="Q63" t="s">
         <v>110</v>
       </c>
-      <c r="Q63">
-        <v>0</v>
-      </c>
       <c r="R63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -4264,29 +4419,29 @@
       <c r="H64" t="s">
         <v>154</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="J64" s="1" t="s">
         <v>196</v>
       </c>
       <c r="L64" t="s">
         <v>172</v>
       </c>
       <c r="M64">
-        <v>0</v>
-      </c>
-      <c r="N64" t="s">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64" t="s">
         <v>160</v>
       </c>
-      <c r="O64" t="s">
-        <v>154</v>
-      </c>
       <c r="P64" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q64" t="s">
         <v>110</v>
       </c>
-      <c r="Q64">
-        <v>1</v>
-      </c>
       <c r="R64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S64">
         <v>2</v>
@@ -4294,8 +4449,11 @@
       <c r="T64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -4320,38 +4478,41 @@
       <c r="H65" t="s">
         <v>154</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="J65" s="1" t="s">
         <v>197</v>
       </c>
       <c r="L65" t="s">
         <v>155</v>
       </c>
       <c r="M65">
-        <v>0</v>
-      </c>
-      <c r="N65" t="s">
+        <v>1</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65" t="s">
         <v>160</v>
       </c>
-      <c r="O65" t="s">
+      <c r="P65" t="s">
         <v>157</v>
       </c>
-      <c r="P65" t="s">
+      <c r="Q65" t="s">
         <v>110</v>
       </c>
-      <c r="Q65">
-        <v>0</v>
-      </c>
       <c r="R65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S65">
         <v>1</v>
       </c>
       <c r="T65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -4376,38 +4537,41 @@
       <c r="H66" t="s">
         <v>154</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="J66" s="1" t="s">
         <v>198</v>
       </c>
       <c r="L66" t="s">
         <v>186</v>
       </c>
       <c r="M66">
-        <v>0</v>
-      </c>
-      <c r="N66" t="s">
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66" t="s">
         <v>160</v>
       </c>
-      <c r="O66" t="s">
-        <v>154</v>
-      </c>
       <c r="P66" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q66" t="s">
         <v>110</v>
       </c>
-      <c r="Q66">
-        <v>1</v>
-      </c>
       <c r="R66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -4432,7 +4596,7 @@
       <c r="H67" t="s">
         <v>154</v>
       </c>
-      <c r="J67" s="2" t="s">
+      <c r="J67" s="1" t="s">
         <v>228</v>
       </c>
       <c r="K67">
@@ -4442,22 +4606,22 @@
         <v>186</v>
       </c>
       <c r="M67">
-        <v>2</v>
-      </c>
-      <c r="N67" t="s">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>2</v>
+      </c>
+      <c r="O67" t="s">
         <v>160</v>
       </c>
-      <c r="O67" t="s">
-        <v>154</v>
-      </c>
       <c r="P67" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q67" t="s">
         <v>111</v>
       </c>
-      <c r="Q67">
-        <v>1</v>
-      </c>
       <c r="R67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S67">
         <v>2</v>
@@ -4465,8 +4629,11 @@
       <c r="T67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -4491,38 +4658,41 @@
       <c r="H68" t="s">
         <v>154</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J68" s="1" t="s">
         <v>199</v>
       </c>
       <c r="L68" t="s">
         <v>186</v>
       </c>
       <c r="M68">
-        <v>0</v>
-      </c>
-      <c r="N68" t="s">
+        <v>1</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68" t="s">
         <v>175</v>
       </c>
-      <c r="O68" t="s">
+      <c r="P68" t="s">
         <v>157</v>
       </c>
-      <c r="P68" t="s">
+      <c r="Q68" t="s">
         <v>111</v>
       </c>
-      <c r="Q68">
-        <v>0</v>
-      </c>
       <c r="R68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S68">
         <v>1</v>
       </c>
       <c r="T68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -4547,7 +4717,7 @@
       <c r="H69" t="s">
         <v>154</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="J69" s="1" t="s">
         <v>200</v>
       </c>
       <c r="L69" t="s">
@@ -4556,18 +4726,18 @@
       <c r="M69">
         <v>0</v>
       </c>
-      <c r="N69" t="s">
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69" t="s">
         <v>160</v>
       </c>
-      <c r="O69" t="s">
+      <c r="P69" t="s">
         <v>157</v>
       </c>
-      <c r="P69" t="s">
+      <c r="Q69" t="s">
         <v>110</v>
       </c>
-      <c r="Q69">
-        <v>1</v>
-      </c>
       <c r="R69">
         <v>1</v>
       </c>
@@ -4575,10 +4745,13 @@
         <v>1</v>
       </c>
       <c r="T69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -4603,38 +4776,41 @@
       <c r="H70" t="s">
         <v>154</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="J70" s="1" t="s">
         <v>201</v>
       </c>
       <c r="L70" t="s">
         <v>186</v>
       </c>
       <c r="M70">
-        <v>1</v>
-      </c>
-      <c r="N70" t="s">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>1</v>
+      </c>
+      <c r="O70" t="s">
         <v>160</v>
       </c>
-      <c r="O70" t="s">
+      <c r="P70" t="s">
         <v>157</v>
       </c>
-      <c r="P70" t="s">
+      <c r="Q70" t="s">
         <v>111</v>
       </c>
-      <c r="Q70">
-        <v>0</v>
-      </c>
-      <c r="R70" t="s">
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70" t="s">
         <v>112</v>
       </c>
-      <c r="S70">
-        <v>1</v>
-      </c>
       <c r="T70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -4659,7 +4835,7 @@
       <c r="H71" t="s">
         <v>154</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="J71" s="1" t="s">
         <v>229</v>
       </c>
       <c r="K71">
@@ -4669,31 +4845,34 @@
         <v>186</v>
       </c>
       <c r="M71">
-        <v>1</v>
-      </c>
-      <c r="N71" t="s">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>1</v>
+      </c>
+      <c r="O71" t="s">
         <v>160</v>
       </c>
-      <c r="O71" t="s">
+      <c r="P71" t="s">
         <v>202</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
         <v>110</v>
       </c>
-      <c r="Q71">
-        <v>0</v>
-      </c>
       <c r="R71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S71">
         <v>1</v>
       </c>
       <c r="T71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -4706,14 +4885,17 @@
       <c r="F72" t="s">
         <v>107</v>
       </c>
-      <c r="P72" t="s">
+      <c r="M72">
+        <v>1</v>
+      </c>
+      <c r="Q72" t="s">
         <v>110</v>
       </c>
-      <c r="Q72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -4738,7 +4920,7 @@
       <c r="H73" t="s">
         <v>154</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="J73" s="1" t="s">
         <v>230</v>
       </c>
       <c r="K73">
@@ -4748,31 +4930,34 @@
         <v>155</v>
       </c>
       <c r="M73">
-        <v>0</v>
-      </c>
-      <c r="N73" t="s">
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73" t="s">
         <v>173</v>
       </c>
-      <c r="O73" t="s">
+      <c r="P73" t="s">
         <v>157</v>
       </c>
-      <c r="P73" t="s">
+      <c r="Q73" t="s">
         <v>111</v>
       </c>
-      <c r="Q73">
-        <v>0</v>
-      </c>
       <c r="R73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T73">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -4797,7 +4982,7 @@
       <c r="H74" t="s">
         <v>154</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="J74" s="1" t="s">
         <v>231</v>
       </c>
       <c r="K74">
@@ -4809,29 +4994,32 @@
       <c r="M74">
         <v>0</v>
       </c>
-      <c r="N74" t="s">
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74" t="s">
         <v>160</v>
       </c>
-      <c r="O74" t="s">
+      <c r="P74" t="s">
         <v>157</v>
       </c>
-      <c r="P74" t="s">
+      <c r="Q74" t="s">
         <v>111</v>
       </c>
-      <c r="Q74">
-        <v>0</v>
-      </c>
-      <c r="R74" t="s">
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74" t="s">
         <v>112</v>
       </c>
-      <c r="S74">
-        <v>1</v>
-      </c>
       <c r="T74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -4856,38 +5044,41 @@
       <c r="H75" t="s">
         <v>154</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="J75" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L75" t="s">
         <v>183</v>
       </c>
       <c r="M75">
-        <v>0</v>
-      </c>
-      <c r="N75" t="s">
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75" t="s">
         <v>160</v>
       </c>
-      <c r="O75" t="s">
+      <c r="P75" t="s">
         <v>157</v>
       </c>
-      <c r="P75" t="s">
+      <c r="Q75" t="s">
         <v>110</v>
       </c>
-      <c r="Q75">
-        <v>0</v>
-      </c>
       <c r="R75">
-        <v>1</v>
-      </c>
-      <c r="S75" t="s">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="T75" t="s">
         <v>112</v>
       </c>
-      <c r="T75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="U75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -4900,14 +5091,14 @@
       <c r="F76" t="s">
         <v>108</v>
       </c>
-      <c r="P76" t="s">
+      <c r="Q76" t="s">
         <v>111</v>
       </c>
-      <c r="Q76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -4920,14 +5111,14 @@
       <c r="F77" t="s">
         <v>108</v>
       </c>
-      <c r="P77" t="s">
+      <c r="Q77" t="s">
         <v>111</v>
       </c>
-      <c r="Q77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -4940,14 +5131,14 @@
       <c r="F78" t="s">
         <v>108</v>
       </c>
-      <c r="P78" t="s">
+      <c r="Q78" t="s">
         <v>110</v>
       </c>
-      <c r="Q78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -4960,14 +5151,14 @@
       <c r="F79" t="s">
         <v>108</v>
       </c>
-      <c r="P79" t="s">
+      <c r="Q79" t="s">
         <v>111</v>
       </c>
-      <c r="Q79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -4980,14 +5171,14 @@
       <c r="F80" t="s">
         <v>108</v>
       </c>
-      <c r="P80" t="s">
+      <c r="Q80" t="s">
         <v>110</v>
       </c>
-      <c r="Q80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -5000,14 +5191,14 @@
       <c r="F81" t="s">
         <v>108</v>
       </c>
-      <c r="P81" t="s">
+      <c r="Q81" t="s">
         <v>111</v>
       </c>
-      <c r="Q81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -5020,14 +5211,14 @@
       <c r="F82" t="s">
         <v>108</v>
       </c>
-      <c r="P82" t="s">
+      <c r="Q82" t="s">
         <v>110</v>
       </c>
-      <c r="Q82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -5040,14 +5231,14 @@
       <c r="F83" t="s">
         <v>108</v>
       </c>
-      <c r="P83" t="s">
+      <c r="Q83" t="s">
         <v>111</v>
       </c>
-      <c r="Q83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -5072,38 +5263,41 @@
       <c r="H84" t="s">
         <v>154</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="J84" s="1" t="s">
         <v>204</v>
       </c>
       <c r="L84" t="s">
         <v>172</v>
       </c>
       <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="N84">
         <v>3</v>
       </c>
-      <c r="N84" t="s">
+      <c r="O84" t="s">
         <v>160</v>
       </c>
-      <c r="O84" t="s">
+      <c r="P84" t="s">
         <v>157</v>
       </c>
-      <c r="P84" t="s">
+      <c r="Q84" t="s">
         <v>110</v>
       </c>
-      <c r="Q84">
-        <v>0</v>
-      </c>
       <c r="R84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S84">
         <v>1</v>
       </c>
       <c r="T84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -5128,7 +5322,7 @@
       <c r="H85" t="s">
         <v>154</v>
       </c>
-      <c r="J85" s="2" t="s">
+      <c r="J85" s="1" t="s">
         <v>205</v>
       </c>
       <c r="L85" t="s">
@@ -5137,18 +5331,18 @@
       <c r="M85">
         <v>0</v>
       </c>
-      <c r="N85" t="s">
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85" t="s">
         <v>206</v>
       </c>
-      <c r="O85" t="s">
+      <c r="P85" t="s">
         <v>157</v>
       </c>
-      <c r="P85" t="s">
+      <c r="Q85" t="s">
         <v>110</v>
       </c>
-      <c r="Q85">
-        <v>1</v>
-      </c>
       <c r="R85">
         <v>1</v>
       </c>
@@ -5156,10 +5350,13 @@
         <v>1</v>
       </c>
       <c r="T85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -5184,38 +5381,41 @@
       <c r="H86" t="s">
         <v>154</v>
       </c>
-      <c r="J86" s="2" t="s">
+      <c r="J86" s="1" t="s">
         <v>207</v>
       </c>
       <c r="L86" t="s">
         <v>172</v>
       </c>
       <c r="M86">
-        <v>0</v>
-      </c>
-      <c r="N86" t="s">
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <v>0</v>
+      </c>
+      <c r="O86" t="s">
         <v>173</v>
       </c>
-      <c r="O86" t="s">
+      <c r="P86" t="s">
         <v>157</v>
       </c>
-      <c r="P86" t="s">
+      <c r="Q86" t="s">
         <v>111</v>
       </c>
-      <c r="Q86">
-        <v>0</v>
-      </c>
       <c r="R86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S86">
         <v>1</v>
       </c>
       <c r="T86">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -5249,29 +5449,32 @@
       <c r="M87">
         <v>0</v>
       </c>
-      <c r="N87" t="s">
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87" t="s">
         <v>165</v>
       </c>
-      <c r="O87" t="s">
+      <c r="P87" t="s">
         <v>157</v>
       </c>
-      <c r="P87" t="s">
+      <c r="Q87" t="s">
         <v>110</v>
       </c>
-      <c r="Q87">
-        <v>1</v>
-      </c>
       <c r="R87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -5296,7 +5499,7 @@
       <c r="H88" t="s">
         <v>154</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="J88" s="1" t="s">
         <v>208</v>
       </c>
       <c r="L88" t="s">
@@ -5305,18 +5508,18 @@
       <c r="M88">
         <v>0</v>
       </c>
-      <c r="N88" t="s">
+      <c r="N88">
+        <v>0</v>
+      </c>
+      <c r="O88" t="s">
         <v>160</v>
       </c>
-      <c r="O88" t="s">
-        <v>154</v>
-      </c>
       <c r="P88" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q88" t="s">
         <v>110</v>
       </c>
-      <c r="Q88">
-        <v>1</v>
-      </c>
       <c r="R88">
         <v>1</v>
       </c>
@@ -5324,10 +5527,13 @@
         <v>1</v>
       </c>
       <c r="T88">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -5352,29 +5558,29 @@
       <c r="H89" t="s">
         <v>154</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="J89" s="1" t="s">
         <v>209</v>
       </c>
       <c r="L89" t="s">
         <v>159</v>
       </c>
       <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89">
         <v>3</v>
       </c>
-      <c r="N89" t="s">
+      <c r="O89" t="s">
         <v>175</v>
       </c>
-      <c r="O89" t="s">
+      <c r="P89" t="s">
         <v>157</v>
       </c>
-      <c r="P89" t="s">
+      <c r="Q89" t="s">
         <v>110</v>
       </c>
-      <c r="Q89">
-        <v>1</v>
-      </c>
       <c r="R89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S89">
         <v>2</v>
@@ -5382,8 +5588,11 @@
       <c r="T89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -5408,7 +5617,7 @@
       <c r="H90" t="s">
         <v>154</v>
       </c>
-      <c r="J90" s="2" t="s">
+      <c r="J90" s="1" t="s">
         <v>232</v>
       </c>
       <c r="K90">
@@ -5418,31 +5627,34 @@
         <v>159</v>
       </c>
       <c r="M90">
-        <v>0</v>
-      </c>
-      <c r="N90" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N90">
+        <v>0</v>
+      </c>
+      <c r="O90" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O90" t="s">
+      <c r="P90" t="s">
         <v>157</v>
       </c>
-      <c r="P90" t="s">
+      <c r="Q90" t="s">
         <v>111</v>
       </c>
-      <c r="Q90">
-        <v>1</v>
-      </c>
       <c r="R90">
         <v>1</v>
       </c>
       <c r="S90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T90">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -5467,38 +5679,41 @@
       <c r="H91" t="s">
         <v>154</v>
       </c>
-      <c r="J91" s="2" t="s">
+      <c r="J91" s="1" t="s">
         <v>210</v>
       </c>
       <c r="L91" t="s">
         <v>166</v>
       </c>
       <c r="M91">
-        <v>0</v>
-      </c>
-      <c r="N91" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N91">
+        <v>0</v>
+      </c>
+      <c r="O91" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O91" t="s">
+      <c r="P91" t="s">
         <v>157</v>
       </c>
-      <c r="P91" t="s">
+      <c r="Q91" t="s">
         <v>110</v>
       </c>
-      <c r="Q91">
-        <v>1</v>
-      </c>
       <c r="R91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S91">
         <v>2</v>
       </c>
       <c r="T91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="U91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -5523,38 +5738,41 @@
       <c r="H92" t="s">
         <v>154</v>
       </c>
-      <c r="J92" s="2" t="s">
+      <c r="J92" s="1" t="s">
         <v>211</v>
       </c>
       <c r="L92" t="s">
         <v>159</v>
       </c>
       <c r="M92">
+        <v>1</v>
+      </c>
+      <c r="N92">
         <v>3</v>
       </c>
-      <c r="N92" t="s">
+      <c r="O92" t="s">
         <v>175</v>
       </c>
-      <c r="O92" t="s">
+      <c r="P92" t="s">
         <v>157</v>
       </c>
-      <c r="P92" t="s">
+      <c r="Q92" t="s">
         <v>110</v>
       </c>
-      <c r="Q92">
-        <v>0</v>
-      </c>
       <c r="R92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S92">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -5579,7 +5797,7 @@
       <c r="H93" t="s">
         <v>154</v>
       </c>
-      <c r="J93" s="2" t="s">
+      <c r="J93" s="1" t="s">
         <v>212</v>
       </c>
       <c r="L93" t="s">
@@ -5588,29 +5806,32 @@
       <c r="M93">
         <v>0</v>
       </c>
-      <c r="N93" t="s">
+      <c r="N93">
+        <v>0</v>
+      </c>
+      <c r="O93" t="s">
         <v>213</v>
       </c>
-      <c r="O93" t="s">
+      <c r="P93" t="s">
         <v>157</v>
       </c>
-      <c r="P93" t="s">
+      <c r="Q93" t="s">
         <v>111</v>
       </c>
-      <c r="Q93">
-        <v>0</v>
-      </c>
       <c r="R93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T93">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -5635,38 +5856,41 @@
       <c r="H94" t="s">
         <v>154</v>
       </c>
-      <c r="J94" s="2" t="s">
+      <c r="J94" s="1" t="s">
         <v>214</v>
       </c>
       <c r="L94" t="s">
         <v>159</v>
       </c>
       <c r="M94">
-        <v>2</v>
-      </c>
-      <c r="N94" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <v>2</v>
+      </c>
+      <c r="O94" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O94" t="s">
+      <c r="P94" t="s">
         <v>157</v>
       </c>
-      <c r="P94" t="s">
+      <c r="Q94" t="s">
         <v>110</v>
       </c>
-      <c r="Q94">
-        <v>0</v>
-      </c>
       <c r="R94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S94">
         <v>1</v>
       </c>
       <c r="T94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -5689,31 +5913,34 @@
         <v>159</v>
       </c>
       <c r="M95">
-        <v>0</v>
-      </c>
-      <c r="N95" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N95">
+        <v>0</v>
+      </c>
+      <c r="O95" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O95" t="s">
+      <c r="P95" t="s">
         <v>157</v>
       </c>
-      <c r="P95" t="s">
+      <c r="Q95" t="s">
         <v>111</v>
       </c>
-      <c r="Q95">
-        <v>1</v>
-      </c>
       <c r="R95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T95">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -5738,38 +5965,41 @@
       <c r="H96" t="s">
         <v>154</v>
       </c>
-      <c r="J96" s="2" t="s">
+      <c r="J96" s="1" t="s">
         <v>215</v>
       </c>
       <c r="L96" t="s">
         <v>159</v>
       </c>
       <c r="M96">
-        <v>1</v>
-      </c>
-      <c r="N96" t="s">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>1</v>
+      </c>
+      <c r="O96" t="s">
         <v>184</v>
       </c>
-      <c r="O96" t="s">
+      <c r="P96" t="s">
         <v>157</v>
       </c>
-      <c r="P96" t="s">
+      <c r="Q96" t="s">
         <v>110</v>
       </c>
-      <c r="Q96">
-        <v>0</v>
-      </c>
       <c r="R96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -5794,45 +6024,42 @@
       <c r="H97" t="s">
         <v>154</v>
       </c>
-      <c r="J97" s="2" t="s">
+      <c r="J97" s="1" t="s">
         <v>216</v>
       </c>
       <c r="L97" t="s">
         <v>159</v>
       </c>
       <c r="M97">
-        <v>2</v>
-      </c>
-      <c r="N97" t="s">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>2</v>
+      </c>
+      <c r="O97" t="s">
         <v>156</v>
       </c>
-      <c r="O97" t="s">
+      <c r="P97" t="s">
         <v>157</v>
       </c>
-      <c r="P97" t="s">
+      <c r="Q97" t="s">
         <v>111</v>
       </c>
-      <c r="Q97">
-        <v>0</v>
-      </c>
-      <c r="R97" t="s">
+      <c r="R97">
+        <v>0</v>
+      </c>
+      <c r="S97" t="s">
         <v>112</v>
       </c>
-      <c r="S97">
-        <v>2</v>
-      </c>
       <c r="T97">
+        <v>2</v>
+      </c>
+      <c r="U97">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T97" xr:uid="{9ADBB74E-D12A-8C49-88BF-474E0A7757AC}">
-    <filterColumn colId="17">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U97" xr:uid="{9ADBB74E-D12A-8C49-88BF-474E0A7757AC}"/>
   <hyperlinks>
     <hyperlink ref="D15" r:id="rId1" xr:uid="{42F51C1E-49FE-F44A-80BE-B1DBE01F57E6}"/>
     <hyperlink ref="D44" r:id="rId2" xr:uid="{635FFB2E-7F06-8448-BD6B-15339C26C7F1}"/>

</xml_diff>